<commit_message>
added modified mainapp.py and MRevidence results in May 24th
</commit_message>
<xml_diff>
--- a/Study_Quality_assessment_MR_BMI_Hypertension.xlsx
+++ b/Study_Quality_assessment_MR_BMI_Hypertension.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qb21134/Library/CloudStorage/OneDrive-UniversityofBristol/Winfred_PhDApps/Streamlit_MRevidenceentryapp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9C763AEB-DEEC-6945-BE55-F2AD94598563}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2F10BC7-5AB7-D84A-A72C-CFC9AF7BE267}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="16020" xr2:uid="{7D774AE9-A5ED-734B-AE9A-9E903EE7B626}"/>
+    <workbookView xWindow="780" yWindow="740" windowWidth="27640" windowHeight="16020" xr2:uid="{7D774AE9-A5ED-734B-AE9A-9E903EE7B626}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="41">
   <si>
     <t>Reference</t>
   </si>
@@ -153,6 +153,12 @@
   </si>
   <si>
     <t>Wes Spiller et al_35947639_2022</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -507,7 +513,7 @@
   <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -562,26 +568,176 @@
       <c r="A2" t="s">
         <v>11</v>
       </c>
+      <c r="B2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J2" t="s">
+        <v>39</v>
+      </c>
+      <c r="K2" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>12</v>
       </c>
+      <c r="B3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H3" t="s">
+        <v>39</v>
+      </c>
+      <c r="I3" t="s">
+        <v>39</v>
+      </c>
+      <c r="J3" t="s">
+        <v>39</v>
+      </c>
+      <c r="K3" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>13</v>
       </c>
+      <c r="B4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" t="s">
+        <v>39</v>
+      </c>
+      <c r="H4" t="s">
+        <v>40</v>
+      </c>
+      <c r="I4" t="s">
+        <v>39</v>
+      </c>
+      <c r="J4" t="s">
+        <v>39</v>
+      </c>
+      <c r="K4" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>14</v>
       </c>
+      <c r="B5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" t="s">
+        <v>39</v>
+      </c>
+      <c r="H5" t="s">
+        <v>40</v>
+      </c>
+      <c r="I5" t="s">
+        <v>39</v>
+      </c>
+      <c r="J5" t="s">
+        <v>39</v>
+      </c>
+      <c r="K5" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>15</v>
       </c>
+      <c r="B6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" t="s">
+        <v>39</v>
+      </c>
+      <c r="H6" t="s">
+        <v>39</v>
+      </c>
+      <c r="I6" t="s">
+        <v>39</v>
+      </c>
+      <c r="J6" t="s">
+        <v>39</v>
+      </c>
+      <c r="K6" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -597,11 +753,71 @@
       <c r="A9" t="s">
         <v>18</v>
       </c>
+      <c r="B9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" t="s">
+        <v>39</v>
+      </c>
+      <c r="G9" t="s">
+        <v>39</v>
+      </c>
+      <c r="H9" t="s">
+        <v>39</v>
+      </c>
+      <c r="I9" t="s">
+        <v>39</v>
+      </c>
+      <c r="J9" t="s">
+        <v>39</v>
+      </c>
+      <c r="K9" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>19</v>
       </c>
+      <c r="B10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" t="s">
+        <v>39</v>
+      </c>
+      <c r="F10" t="s">
+        <v>39</v>
+      </c>
+      <c r="G10" t="s">
+        <v>39</v>
+      </c>
+      <c r="H10" t="s">
+        <v>39</v>
+      </c>
+      <c r="I10" t="s">
+        <v>39</v>
+      </c>
+      <c r="J10" t="s">
+        <v>39</v>
+      </c>
+      <c r="K10" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -633,69 +849,159 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" t="s">
+        <v>39</v>
+      </c>
+      <c r="E20" t="s">
+        <v>39</v>
+      </c>
+      <c r="F20" t="s">
+        <v>39</v>
+      </c>
+      <c r="G20" t="s">
+        <v>39</v>
+      </c>
+      <c r="H20" t="s">
+        <v>39</v>
+      </c>
+      <c r="I20" t="s">
+        <v>39</v>
+      </c>
+      <c r="J20" t="s">
+        <v>39</v>
+      </c>
+      <c r="K20" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" t="s">
+        <v>39</v>
+      </c>
+      <c r="D22" t="s">
+        <v>39</v>
+      </c>
+      <c r="E22" t="s">
+        <v>39</v>
+      </c>
+      <c r="F22" t="s">
+        <v>39</v>
+      </c>
+      <c r="G22" t="s">
+        <v>39</v>
+      </c>
+      <c r="H22" t="s">
+        <v>39</v>
+      </c>
+      <c r="I22" t="s">
+        <v>39</v>
+      </c>
+      <c r="J22" t="s">
+        <v>39</v>
+      </c>
+      <c r="K22" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>38</v>
+      </c>
+      <c r="B29" t="s">
+        <v>39</v>
+      </c>
+      <c r="C29" t="s">
+        <v>39</v>
+      </c>
+      <c r="D29" t="s">
+        <v>39</v>
+      </c>
+      <c r="E29" t="s">
+        <v>39</v>
+      </c>
+      <c r="F29" t="s">
+        <v>39</v>
+      </c>
+      <c r="G29" t="s">
+        <v>39</v>
+      </c>
+      <c r="H29" t="s">
+        <v>40</v>
+      </c>
+      <c r="I29" t="s">
+        <v>39</v>
+      </c>
+      <c r="J29" t="s">
+        <v>39</v>
+      </c>
+      <c r="K29" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>